<commit_message>
Edit minor error in xlsx
</commit_message>
<xml_diff>
--- a/CS2101_G04.xlsx
+++ b/CS2101_G04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neoru\Documents\NUS\Y2S1\CS2103T\Team Project\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC555A7C-390C-4D05-92CB-041FD79BD99E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06F6E63-ECAE-4F49-8C36-5C6DCBFB194C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>T6</t>
   </si>
   <si>
-    <t xml:space="preserve">     T7</t>
-  </si>
-  <si>
     <t>BU WEN JIN</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>A0205306U</t>
+  </si>
+  <si>
+    <t>T7</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,18 +921,18 @@
       <c r="I5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="15" t="s">
-        <v>11</v>
+      <c r="J5" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
       <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="17">
         <v>1</v>
@@ -960,10 +960,10 @@
     <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="17">
         <v>1</v>
@@ -991,10 +991,10 @@
     <row r="8" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="17">
         <v>1</v>
@@ -1022,10 +1022,10 @@
     <row r="9" spans="1:11" ht="35.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="17">
         <v>1</v>
@@ -1053,10 +1053,10 @@
     <row r="10" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16"/>
       <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>

</xml_diff>

<commit_message>
change excel sheet details
</commit_message>
<xml_diff>
--- a/CS2101_G04.xlsx
+++ b/CS2101_G04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neoru\Documents\NUS\Y2S1\CS2103T\Team Project\tp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darea\Documents\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06F6E63-ECAE-4F49-8C36-5C6DCBFB194C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E74BE6-CA03-432F-BB71-DADBC59ED5DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,34 +71,34 @@
     <t>BU WEN JIN</t>
   </si>
   <si>
-    <t>A0205129M</t>
-  </si>
-  <si>
     <t>LAU XIN YEE</t>
   </si>
   <si>
-    <t>A0204878U</t>
-  </si>
-  <si>
     <t>LIM CHUN YONG</t>
   </si>
   <si>
-    <t>A0199902R</t>
-  </si>
-  <si>
     <t>LIM JIA RUI RYAN</t>
   </si>
   <si>
-    <t>A0199815L</t>
-  </si>
-  <si>
     <t>NEO RUI EN MAYBELLINE</t>
   </si>
   <si>
-    <t>A0205306U</t>
-  </si>
-  <si>
     <t>T7</t>
+  </si>
+  <si>
+    <t>A01234567M</t>
+  </si>
+  <si>
+    <t>A07654321U</t>
+  </si>
+  <si>
+    <t>A03884431R</t>
+  </si>
+  <si>
+    <t>A05873124L</t>
+  </si>
+  <si>
+    <t>A0139345U</t>
   </si>
 </sst>
 </file>
@@ -296,14 +296,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>338137</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>21648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>52386</xdr:rowOff>
+      <xdr:colOff>326409</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>321944</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -319,15 +319,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1062037"/>
-          <a:ext cx="285750" cy="381000"/>
+          <a:off x="0" y="974148"/>
+          <a:ext cx="326409" cy="300296"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -339,15 +344,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>25977</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28116</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>489238</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
+      <xdr:rowOff>338037</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -363,15 +368,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1471613"/>
-          <a:ext cx="285750" cy="381000"/>
+          <a:off x="25977" y="1305332"/>
+          <a:ext cx="463261" cy="309921"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -383,15 +393,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>97971</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>10886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>346389</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:rowOff>11468</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -407,15 +417,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1838325"/>
-          <a:ext cx="285750" cy="381000"/>
+          <a:off x="97971" y="1681843"/>
+          <a:ext cx="248418" cy="316268"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -429,13 +444,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>58534</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
+      <xdr:colOff>441614</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>18877</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -451,15 +466,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2233613"/>
-          <a:ext cx="285750" cy="381000"/>
+          <a:off x="0" y="2041466"/>
+          <a:ext cx="441614" cy="406286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -471,15 +491,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>27214</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>32657</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
+      <xdr:colOff>471812</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>33474</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -495,15 +515,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2652713"/>
-          <a:ext cx="285750" cy="381000"/>
+          <a:off x="27214" y="2465614"/>
+          <a:ext cx="444598" cy="409031"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -814,17 +839,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A562E69-3C8B-494C-84C7-9127BBCE2717}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +866,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="4"/>
@@ -854,7 +879,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="5"/>
@@ -866,7 +891,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -893,7 +918,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -922,17 +947,17 @@
         <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D6" s="17">
         <v>1</v>
@@ -957,13 +982,13 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D7" s="17">
         <v>1</v>
@@ -988,13 +1013,13 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D8" s="17">
         <v>1</v>
@@ -1019,13 +1044,13 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="35.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="35.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="17">
         <v>1</v>
@@ -1050,13 +1075,13 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>

</xml_diff>

<commit_message>
Revert "Load default group if no data available"
This reverts commit 3b7d34bf5a7b5093286d935ce2b5f26661acbc2c.
</commit_message>
<xml_diff>
--- a/CS2101_G04.xlsx
+++ b/CS2101_G04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darea\Documents\tp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neoru\Documents\NUS\Y2S1\CS2103T\Team Project\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312DB1AD-E906-4B9D-A4F2-5CA97AC65DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06F6E63-ECAE-4F49-8C36-5C6DCBFB194C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>CS2101 (2010 - 2020/2021 Semester 1) G09</t>
   </si>
@@ -71,40 +71,34 @@
     <t>BU WEN JIN</t>
   </si>
   <si>
+    <t>A0205129M</t>
+  </si>
+  <si>
     <t>LAU XIN YEE</t>
   </si>
   <si>
+    <t>A0204878U</t>
+  </si>
+  <si>
     <t>LIM CHUN YONG</t>
   </si>
   <si>
+    <t>A0199902R</t>
+  </si>
+  <si>
     <t>LIM JIA RUI RYAN</t>
   </si>
   <si>
+    <t>A0199815L</t>
+  </si>
+  <si>
     <t>NEO RUI EN MAYBELLINE</t>
   </si>
   <si>
+    <t>A0205306U</t>
+  </si>
+  <si>
     <t>T7</t>
-  </si>
-  <si>
-    <t>A01234567M</t>
-  </si>
-  <si>
-    <t>A07654321U</t>
-  </si>
-  <si>
-    <t>A03884431R</t>
-  </si>
-  <si>
-    <t>A05873124L</t>
-  </si>
-  <si>
-    <t>A0139345U</t>
-  </si>
-  <si>
-    <t>AARON TAN</t>
-  </si>
-  <si>
-    <t>A33333333S</t>
   </si>
 </sst>
 </file>
@@ -246,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -279,10 +273,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -306,14 +296,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>21648</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>338137</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>326409</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>321944</xdr:rowOff>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -329,20 +319,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="974148"/>
-          <a:ext cx="326409" cy="300296"/>
+          <a:off x="0" y="1062037"/>
+          <a:ext cx="285750" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -354,15 +339,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>25977</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28116</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>489238</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>338037</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -378,20 +363,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25977" y="1305332"/>
-          <a:ext cx="463261" cy="309921"/>
+          <a:off x="0" y="1471613"/>
+          <a:ext cx="285750" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -403,15 +383,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>97971</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>346389</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>11468</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -427,20 +407,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="97971" y="1681843"/>
-          <a:ext cx="248418" cy="316268"/>
+          <a:off x="0" y="1838325"/>
+          <a:ext cx="285750" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -453,14 +428,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>58534</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>441614</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>18877</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -476,20 +451,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2041466"/>
-          <a:ext cx="441614" cy="406286"/>
+          <a:off x="0" y="2233613"/>
+          <a:ext cx="285750" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -501,15 +471,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>471812</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>33474</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -525,69 +495,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27214" y="2465614"/>
-          <a:ext cx="444598" cy="409031"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27215</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>157719</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>353624</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>77015</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="e69c3e4d-a819-41dd-9585-6e67411ad498">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00F3DAA2-BE4B-4E5B-B898-9DF86917FE71}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27215" y="919719"/>
-          <a:ext cx="326409" cy="300296"/>
+          <a:off x="0" y="2652713"/>
+          <a:ext cx="285750" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -896,19 +812,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A562E69-3C8B-494C-84C7-9127BBCE2717}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +841,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="4"/>
@@ -938,7 +854,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="5"/>
@@ -950,7 +866,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -977,7 +893,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -1006,48 +922,48 @@
         <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="19">
-        <v>1</v>
-      </c>
-      <c r="E6" s="19">
-        <v>1</v>
-      </c>
-      <c r="F6" s="19">
-        <v>1</v>
-      </c>
-      <c r="G6" s="19">
-        <v>1</v>
-      </c>
-      <c r="H6" s="19">
-        <v>1</v>
-      </c>
-      <c r="I6" s="19">
-        <v>1</v>
-      </c>
-      <c r="J6" s="19">
-        <v>1</v>
-      </c>
-      <c r="K6" s="15"/>
+    <row r="6" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16"/>
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="17">
+        <v>1</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1</v>
+      </c>
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
+      <c r="I6" s="17">
+        <v>1</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" s="17">
         <v>1</v>
@@ -1072,13 +988,13 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="17">
         <v>1</v>
@@ -1103,13 +1019,13 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="35.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="17">
         <v>1</v>
@@ -1134,10 +1050,10 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="35.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16"/>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>20</v>
@@ -1164,41 +1080,9 @@
         <v>1</v>
       </c>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="17">
-        <v>1</v>
-      </c>
-      <c r="E11" s="17">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17">
-        <v>1</v>
-      </c>
-      <c r="G11" s="17">
-        <v>1</v>
-      </c>
-      <c r="H11" s="17">
-        <v>1</v>
-      </c>
-      <c r="I11" s="17">
-        <v>1</v>
-      </c>
-      <c r="J11" s="17">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reduce studentNo in excel sheet to 9 characters long
</commit_message>
<xml_diff>
--- a/CS2101_G04.xlsx
+++ b/CS2101_G04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darea\Documents\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312DB1AD-E906-4B9D-A4F2-5CA97AC65DB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD61D600-B4F2-4292-97E7-7D9F1752A977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
   </bookViews>
@@ -86,25 +86,25 @@
     <t>T7</t>
   </si>
   <si>
-    <t>A01234567M</t>
-  </si>
-  <si>
-    <t>A07654321U</t>
-  </si>
-  <si>
-    <t>A03884431R</t>
-  </si>
-  <si>
-    <t>A05873124L</t>
-  </si>
-  <si>
     <t>A0139345U</t>
   </si>
   <si>
     <t>AARON TAN</t>
   </si>
   <si>
-    <t>A33333333S</t>
+    <t>A3333333S</t>
+  </si>
+  <si>
+    <t>A0123456M</t>
+  </si>
+  <si>
+    <t>A0765432U</t>
+  </si>
+  <si>
+    <t>A0388443R</t>
+  </si>
+  <si>
+    <t>A0587314L</t>
   </si>
 </sst>
 </file>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A562E69-3C8B-494C-84C7-9127BBCE2717}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,10 +1013,10 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" s="19">
         <v>1</v>
@@ -1047,7 +1047,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" s="17">
         <v>1</v>
@@ -1078,7 +1078,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D8" s="17">
         <v>1</v>
@@ -1109,7 +1109,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D9" s="17">
         <v>1</v>
@@ -1140,7 +1140,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>
@@ -1171,7 +1171,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D11" s="17">
         <v>1</v>

</xml_diff>

<commit_message>
Change A3333333S to A0123456U in CS2101_G04.xlsx
</commit_message>
<xml_diff>
--- a/CS2101_G04.xlsx
+++ b/CS2101_G04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darea\Documents\tp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neoru\Documents\NUS\Y2S1\CS2103T\Team Project\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD61D600-B4F2-4292-97E7-7D9F1752A977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566184A9-39AA-4163-83E2-2277E5B4AE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{421CD01B-00FF-4255-A315-0A58B00F9296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>AARON TAN</t>
   </si>
   <si>
-    <t>A3333333S</t>
-  </si>
-  <si>
     <t>A0123456M</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>A0587314L</t>
+  </si>
+  <si>
+    <t>A0123456U</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -899,16 +899,16 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="4"/>
@@ -938,7 +938,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="5"/>
@@ -950,7 +950,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -977,7 +977,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -1010,13 +1010,13 @@
       </c>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" s="19">
         <v>1</v>
@@ -1041,13 +1041,13 @@
       </c>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="17">
         <v>1</v>
@@ -1072,13 +1072,13 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="17">
         <v>1</v>
@@ -1103,13 +1103,13 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="17">
         <v>1</v>
@@ -1134,13 +1134,13 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="35.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="35.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16"/>
       <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
       <c r="B11" s="6" t="s">
         <v>15</v>

</xml_diff>